<commit_message>
Modified IS & BS xlsx - CFC added
</commit_message>
<xml_diff>
--- a/Specs/IS & BS.xlsx
+++ b/Specs/IS & BS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>EBIT</t>
   </si>
@@ -117,9 +117,6 @@
     <t>hlp</t>
   </si>
   <si>
-    <t>day of project start</t>
-  </si>
-  <si>
     <t>decrease of short term loans</t>
   </si>
   <si>
@@ -127,6 +124,15 @@
   </si>
   <si>
     <t>minimal cash balance</t>
+  </si>
+  <si>
+    <t>FCF project</t>
+  </si>
+  <si>
+    <t>FCF owners</t>
+  </si>
+  <si>
+    <t>day 1 of project start</t>
   </si>
 </sst>
 </file>
@@ -318,8 +324,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,7 +412,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -412,6 +420,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -419,6 +428,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:H41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1130,7 +1140,7 @@
     </row>
     <row r="18" spans="1:8" ht="37" thickBot="1">
       <c r="B18" s="22" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="16" thickBot="1">
@@ -1146,7 +1156,7 @@
         <v>10000</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" ref="B19:H19" si="8">D20</f>
+        <f t="shared" ref="D19:H19" si="8">D20</f>
         <v>9000</v>
       </c>
       <c r="E19" s="10">
@@ -1181,19 +1191,19 @@
         <v>9000</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" ref="E20:H20" si="9">D20-E9</f>
+        <f>D20-E9</f>
         <v>8000</v>
       </c>
       <c r="F20" s="14">
-        <f t="shared" si="9"/>
+        <f>E20-F9</f>
         <v>7000</v>
       </c>
       <c r="G20" s="14">
-        <f t="shared" si="9"/>
+        <f>F20-G9</f>
         <v>6000</v>
       </c>
       <c r="H20" s="14">
-        <f t="shared" si="9"/>
+        <f>G20-H9</f>
         <v>5000</v>
       </c>
     </row>
@@ -1202,31 +1212,31 @@
         <v>9</v>
       </c>
       <c r="B21" s="10">
-        <f t="shared" ref="B21:H21" si="10">SUM(B22:B24)</f>
-        <v>2000</v>
+        <f t="shared" ref="B21:H21" si="9">SUM(B22:B24)</f>
+        <v>0</v>
       </c>
       <c r="C21" s="10">
-        <f t="shared" si="10"/>
-        <v>916.66666666666674</v>
+        <f t="shared" si="9"/>
+        <v>916.66666666666663</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" si="10"/>
-        <v>1276.6666666666667</v>
+        <f t="shared" si="9"/>
+        <v>1276.6666666666665</v>
       </c>
       <c r="E21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>833.33333333333326</v>
       </c>
       <c r="F21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>833.33333333333326</v>
       </c>
       <c r="G21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1683.0826666666665</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>2243.0826666666662</v>
       </c>
     </row>
@@ -1292,30 +1302,30 @@
         <v>12</v>
       </c>
       <c r="B24" s="12">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C24" s="14">
-        <f t="shared" ref="C24:H24" si="11">B24-C41</f>
-        <v>916.66666666666674</v>
+        <f>B24-C41</f>
+        <v>916.66666666666663</v>
       </c>
       <c r="D24" s="14">
-        <f t="shared" si="11"/>
-        <v>943.33333333333337</v>
+        <f t="shared" ref="D24:H24" si="10">C24-D41</f>
+        <v>943.33333333333326</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>500</v>
       </c>
       <c r="F24" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>500</v>
       </c>
       <c r="G24" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1349.7493333333332</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1909.7493333333327</v>
       </c>
     </row>
@@ -1324,31 +1334,31 @@
         <v>7</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" ref="B25" si="12">B19+B21</f>
-        <v>2000</v>
+        <f t="shared" ref="B25" si="11">B19+B21</f>
+        <v>0</v>
       </c>
       <c r="C25" s="10">
-        <f t="shared" ref="C25:H25" si="13">C19+C21</f>
+        <f t="shared" ref="C25:H25" si="12">C19+C21</f>
         <v>10916.666666666666</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>10276.666666666666</v>
       </c>
       <c r="E25" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>8833.3333333333339</v>
       </c>
       <c r="F25" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7833.333333333333</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7683.0826666666662</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7243.0826666666662</v>
       </c>
     </row>
@@ -1358,7 +1368,7 @@
       </c>
       <c r="B26" s="10">
         <f>SUM(B27:B29)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C26" s="10">
         <f>SUM(C27:C29)</f>
@@ -1369,19 +1379,19 @@
         <v>2260</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" ref="E26:H26" si="14">SUM(E27:E29)</f>
+        <f t="shared" ref="E26:H26" si="13">SUM(E27:E29)</f>
         <v>2660</v>
       </c>
       <c r="F26" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3133.7333333333331</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3666.4159999999997</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>4226.4159999999993</v>
       </c>
     </row>
@@ -1390,7 +1400,8 @@
         <v>13</v>
       </c>
       <c r="B27" s="12">
-        <v>2000</v>
+        <f>B24</f>
+        <v>0</v>
       </c>
       <c r="C27" s="12">
         <v>2000</v>
@@ -1400,19 +1411,19 @@
         <v>2000</v>
       </c>
       <c r="E27" s="12">
-        <f t="shared" ref="E27:H27" si="15">D27</f>
+        <f t="shared" ref="E27:H27" si="14">D27</f>
         <v>2000</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
     </row>
@@ -1421,31 +1432,31 @@
         <v>17</v>
       </c>
       <c r="B28" s="14">
-        <f t="shared" ref="B28" si="16">B14</f>
+        <f t="shared" ref="B28" si="15">B14</f>
         <v>0</v>
       </c>
       <c r="C28" s="14">
-        <f t="shared" ref="C28:H28" si="17">C14</f>
+        <f>C14</f>
         <v>-100</v>
       </c>
       <c r="D28" s="14">
-        <f t="shared" si="17"/>
+        <f>D14</f>
         <v>360</v>
       </c>
       <c r="E28" s="14">
-        <f t="shared" si="17"/>
+        <f>E14</f>
         <v>400</v>
       </c>
       <c r="F28" s="14">
-        <f t="shared" si="17"/>
+        <f>F14</f>
         <v>473.73333333333323</v>
       </c>
       <c r="G28" s="14">
-        <f t="shared" si="17"/>
+        <f>G14</f>
         <v>532.68266666666671</v>
       </c>
       <c r="H28" s="14">
-        <f t="shared" si="17"/>
+        <f>H14</f>
         <v>560</v>
       </c>
     </row>
@@ -1463,19 +1474,19 @@
         <v>-100</v>
       </c>
       <c r="E29" s="14">
-        <f t="shared" ref="E29:H29" si="18">D29+D28</f>
+        <f t="shared" ref="E29:H29" si="16">D29+D28</f>
         <v>260</v>
       </c>
       <c r="F29" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>660</v>
       </c>
       <c r="G29" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1133.7333333333331</v>
       </c>
       <c r="H29" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1666.4159999999997</v>
       </c>
     </row>
@@ -1484,31 +1495,31 @@
         <v>14</v>
       </c>
       <c r="B30" s="10">
-        <f t="shared" ref="B30:H30" si="19">SUM(B31:B33)</f>
+        <f t="shared" ref="B30:H30" si="17">SUM(B31:B33)</f>
         <v>0</v>
       </c>
       <c r="C30" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>9016.6666666666661</v>
       </c>
       <c r="D30" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>8016.666666666667</v>
       </c>
       <c r="E30" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>6173.3333333333348</v>
       </c>
       <c r="F30" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>4699.6000000000004</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>4016.6666666666665</v>
       </c>
       <c r="H30" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>3016.6666666666665</v>
       </c>
     </row>
@@ -1546,31 +1557,31 @@
         <v>0</v>
       </c>
       <c r="C32" s="14">
-        <f t="shared" ref="C32:H32" si="20">B32-C39</f>
+        <f>B32-C39</f>
         <v>0</v>
       </c>
       <c r="D32" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="D32:H32" si="18">C32-D39</f>
         <v>0</v>
       </c>
       <c r="E32" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1156.6666666666679</v>
       </c>
       <c r="F32" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2682.9333333333334</v>
       </c>
       <c r="G32" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H32" s="14">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="12" t="s">
         <v>22</v>
       </c>
@@ -1584,147 +1595,147 @@
         <v>16.666666666666668</v>
       </c>
       <c r="E33" s="23">
-        <f t="shared" ref="E33:H33" si="21">E5/6</f>
+        <f>E5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="F33" s="23">
-        <f t="shared" si="21"/>
+        <f>F5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="G33" s="23">
-        <f t="shared" si="21"/>
+        <f>G5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="H33" s="23">
-        <f t="shared" si="21"/>
+        <f>H5/6</f>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="16" thickBot="1">
+    <row r="34" spans="1:9" ht="16" thickBot="1">
       <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="10">
-        <f t="shared" ref="B34" si="22">B26+B30</f>
-        <v>2000</v>
+        <f t="shared" ref="B34" si="19">B26+B30</f>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <f t="shared" ref="C34:H34" si="23">C26+C30</f>
+        <f t="shared" ref="C34:H34" si="20">C26+C30</f>
         <v>10916.666666666666</v>
       </c>
       <c r="D34" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>10276.666666666668</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>8833.3333333333358</v>
       </c>
       <c r="F34" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>7833.3333333333339</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>7683.0826666666662</v>
       </c>
       <c r="H34" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>7243.0826666666653</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="16">
-        <f t="shared" ref="B35:H35" si="24">B25-B34</f>
+        <f t="shared" ref="B35:H35" si="21">B25-B34</f>
         <v>0</v>
       </c>
       <c r="C35" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="D35" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="E35" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F35" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G35" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H35" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="16">
         <f>C19+C22+C23+B24-C26-C31-B32-C33</f>
-        <v>1083.3333333333333</v>
+        <v>-916.66666666666663</v>
       </c>
       <c r="D38" s="16">
         <f>D19+D22+D23+C24-D26-D31-C32-D33</f>
         <v>-26.666666666666668</v>
       </c>
       <c r="E38" s="16">
-        <f t="shared" ref="E38:H38" si="25">E19+E22+E23+D24-E26-E31-D32-E33</f>
+        <f t="shared" ref="E38:H38" si="22">E19+E22+E23+D24-E26-E31-D32-E33</f>
         <v>1600.0000000000011</v>
       </c>
       <c r="F38" s="16">
+        <f t="shared" si="22"/>
+        <v>1526.2666666666657</v>
+      </c>
+      <c r="G38" s="16">
+        <f t="shared" si="22"/>
+        <v>-3532.6826666666666</v>
+      </c>
+      <c r="H38" s="16">
+        <f t="shared" si="22"/>
+        <v>-559.99999999999966</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="16">
+        <f>IF(C38&gt;=0,MIN(B32,-C38+MAX(C41,0)),MIN(B32,-C38))</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" ref="D39" si="23">IF(D38&gt;=0,MIN(C32,-D38+MAX(D41,0)),MIN(C32,-D38))</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <f t="shared" ref="E39" si="24">IF(E38&gt;=0,MIN(D32,-E38+MAX(E41,0)),MIN(D32,-E38))</f>
+        <v>-1156.6666666666679</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" ref="F39:H39" si="25">IF(F38&gt;=0,MIN(E32,-F38+MAX(F41,0)),MIN(E32,-F38))</f>
+        <v>-1526.2666666666657</v>
+      </c>
+      <c r="G39" s="16">
         <f t="shared" si="25"/>
-        <v>1526.2666666666657</v>
-      </c>
-      <c r="G38" s="16">
+        <v>2682.9333333333334</v>
+      </c>
+      <c r="H39" s="16">
         <f t="shared" si="25"/>
-        <v>-3532.6826666666666</v>
-      </c>
-      <c r="H38" s="16">
-        <f t="shared" si="25"/>
-        <v>-559.99999999999966</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="16">
-        <f t="shared" ref="C39" si="26">IF(C38&gt;=0,MIN(B32,-C38+MAX(C41,0)),MIN(B32,-C38))</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="16">
-        <f t="shared" ref="D39" si="27">IF(D38&gt;=0,MIN(C32,-D38+MAX(D41,0)),MIN(C32,-D38))</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="16">
-        <f t="shared" ref="E39" si="28">IF(E38&gt;=0,MIN(D32,-E38+MAX(E41,0)),MIN(D32,-E38))</f>
-        <v>-1156.6666666666679</v>
-      </c>
-      <c r="F39" s="16">
-        <f t="shared" ref="E39:H39" si="29">IF(F38&gt;=0,MIN(E32,-F38+MAX(F41,0)),MIN(E32,-F38))</f>
-        <v>-1526.2666666666657</v>
-      </c>
-      <c r="G39" s="16">
-        <f t="shared" si="29"/>
-        <v>2682.9333333333334</v>
-      </c>
-      <c r="H39" s="16">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1732,42 +1743,106 @@
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="16">
+        <f>IF(C38&gt;=0,MIN(C38,B24-$C$43),(C38+C39))</f>
+        <v>-916.66666666666663</v>
+      </c>
+      <c r="D41" s="16">
+        <f>IF(D38&gt;=0,MIN(D38,C24-$C$43),(D38+D39))</f>
+        <v>-26.666666666666668</v>
+      </c>
+      <c r="E41" s="16">
+        <f>IF(E38&gt;=0,MIN(E38,D24-$C$43),(E38+E39))</f>
+        <v>443.33333333333326</v>
+      </c>
+      <c r="F41" s="16">
+        <f>IF(F38&gt;=0,MIN(F38,E24-$C$43),(F38+F39))</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <f>IF(G38&gt;=0,MIN(G38,F24-$C$43),(G38+G39))</f>
+        <v>-849.7493333333332</v>
+      </c>
+      <c r="H41" s="16">
+        <f>IF(H38&gt;=0,MIN(H38,G24-$C$43),(H38+H39))</f>
+        <v>-559.99999999999966</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="16">
-        <f>IF(C38&gt;=0,MIN(C38,B24-$B$43),(C38+C39))</f>
-        <v>1083.3333333333333</v>
-      </c>
-      <c r="D41" s="16">
-        <f t="shared" ref="D41:H41" si="30">IF(D38&gt;=0,MIN(D38,C24-$B$43),(D38+D39))</f>
-        <v>-26.666666666666668</v>
-      </c>
-      <c r="E41" s="16">
-        <f t="shared" si="30"/>
-        <v>443.33333333333337</v>
-      </c>
-      <c r="F41" s="16">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="G41" s="16">
-        <f t="shared" si="30"/>
-        <v>-849.7493333333332</v>
-      </c>
-      <c r="H41" s="16">
-        <f t="shared" si="30"/>
-        <v>-559.99999999999966</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="24" t="s">
+      <c r="C43" s="24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="24">
-        <v>500</v>
-      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16">
+        <f>C14-(C20-B20)-(C22-B22)+(C33-B33)+C11-C24</f>
+        <v>-11000</v>
+      </c>
+      <c r="D46" s="16">
+        <f>D14-(D20-C20)-(D22-C22)+(D33-C33)+D11</f>
+        <v>1476.6666666666667</v>
+      </c>
+      <c r="E46" s="16">
+        <f>E14-(E20-D20)-(E22-D22)+(E33-D33)+E11</f>
+        <v>1800</v>
+      </c>
+      <c r="F46" s="16">
+        <f>F14-(F20-E20)-(F22-E22)+(F33-E33)+F11</f>
+        <v>1781.5666666666666</v>
+      </c>
+      <c r="G46" s="16">
+        <f>G14-(G20-F20)-(G22-F22)+(G33-F33)+G11</f>
+        <v>1766.8293333333334</v>
+      </c>
+      <c r="H46" s="16">
+        <f>H14-(H20-G20)-(H22-G22)+(H33-G33)+H11</f>
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16">
+        <f>-(C27-B27)+C14+C9</f>
+        <v>-2100</v>
+      </c>
+      <c r="D47" s="16">
+        <f>-(D27-C27)-D41</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="E47" s="16">
+        <f t="shared" ref="E47:H47" si="26">-(E27-D27)-E41</f>
+        <v>-443.33333333333326</v>
+      </c>
+      <c r="F47" s="16">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <f t="shared" si="26"/>
+        <v>849.7493333333332</v>
+      </c>
+      <c r="H47" s="16">
+        <f t="shared" si="26"/>
+        <v>559.99999999999966</v>
+      </c>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add irr calculation, add yearly reports
</commit_message>
<xml_diff>
--- a/Specs/IS & BS.xlsx
+++ b/Specs/IS & BS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="15870" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" iterate="1" iterateCount="1000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>EBIT</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>day 1 of project start</t>
+  </si>
+  <si>
+    <t>fixed_assets+Operating Receivables + Short-Term Investments-  Equity - Lt_dept- St_dept_supl + PREVIOUS(Assets On Bank Accounts - ST_loans)</t>
+  </si>
+  <si>
+    <t>C14-(C20-B20)-(C22-B22)+(C33-B33)+C11-C24</t>
+  </si>
+  <si>
+    <t>Net earnings - CP_fixed_assets  - CP_Operating Receivables + CP_Short-Term Debt to Suppliers+C_Interests Paid-C_Assets On Bank Accounts</t>
+  </si>
+  <si>
+    <t>-(C27-B27)+C14+C9</t>
+  </si>
+  <si>
+    <t>- CP_Paid-In Capital+C_net_earn+C_Deprication</t>
   </si>
 </sst>
 </file>
@@ -185,11 +200,15 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -343,7 +362,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -411,28 +430,36 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -758,19 +785,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:H47"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="40.875" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -792,7 +819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -822,7 +849,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
@@ -844,7 +871,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>25</v>
       </c>
@@ -866,7 +893,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
@@ -896,7 +923,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -910,7 +937,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -932,7 +959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -962,7 +989,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -984,7 +1011,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1041,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1071,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -1074,7 +1101,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -1104,7 +1131,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1134,16 +1161,16 @@
         <v>560</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
     </row>
-    <row r="18" spans="1:8" ht="37" thickBot="1">
+    <row r="18" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16" thickBot="1">
+    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>8</v>
       </c>
@@ -1176,7 +1203,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16" thickBot="1">
+    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>30</v>
       </c>
@@ -1207,17 +1234,17 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16" thickBot="1">
+    <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="10">
         <f t="shared" ref="B21:H21" si="9">SUM(B22:B24)</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="C21" s="10">
         <f t="shared" si="9"/>
-        <v>916.66666666666663</v>
+        <v>916.66666666666652</v>
       </c>
       <c r="D21" s="10">
         <f t="shared" si="9"/>
@@ -1240,7 +1267,7 @@
         <v>2243.0826666666662</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>10</v>
       </c>
@@ -1271,7 +1298,7 @@
         <v>333.33333333333331</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>11</v>
       </c>
@@ -1297,78 +1324,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16" thickBot="1">
+    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="12">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="C24" s="14">
-        <f>B24-C41</f>
-        <v>916.66666666666663</v>
+        <f>B24-C46</f>
+        <v>916.66666666666652</v>
       </c>
       <c r="D24" s="14">
-        <f t="shared" ref="D24:H24" si="10">C24-D41</f>
-        <v>943.33333333333326</v>
+        <f>C24-D46</f>
+        <v>943.33333333333314</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" si="10"/>
+        <f>D24-E46</f>
         <v>500</v>
       </c>
       <c r="F24" s="14">
-        <f t="shared" si="10"/>
+        <f>E24-F46</f>
         <v>500</v>
       </c>
       <c r="G24" s="14">
-        <f t="shared" si="10"/>
+        <f>F24-G46</f>
         <v>1349.7493333333332</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" si="10"/>
+        <f>G24-H46</f>
         <v>1909.7493333333327</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16" thickBot="1">
+    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" ref="B25" si="11">B19+B21</f>
-        <v>0</v>
+        <f t="shared" ref="B25" si="10">B19+B21</f>
+        <v>2000</v>
       </c>
       <c r="C25" s="10">
-        <f t="shared" ref="C25:H25" si="12">C19+C21</f>
+        <f t="shared" ref="C25:H25" si="11">C19+C21</f>
         <v>10916.666666666666</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>10276.666666666666</v>
       </c>
       <c r="E25" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8833.3333333333339</v>
       </c>
       <c r="F25" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7833.333333333333</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7683.0826666666662</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7243.0826666666662</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16" thickBot="1">
+    <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="10">
         <f>SUM(B27:B29)</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="C26" s="10">
         <f>SUM(C27:C29)</f>
@@ -1379,29 +1406,28 @@
         <v>2260</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" ref="E26:H26" si="13">SUM(E27:E29)</f>
+        <f t="shared" ref="E26:H26" si="12">SUM(E27:E29)</f>
         <v>2660</v>
       </c>
       <c r="F26" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3133.7333333333331</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3666.4159999999997</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4226.4159999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="12">
-        <f>B24</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="C27" s="12">
         <v>2000</v>
@@ -1411,56 +1437,56 @@
         <v>2000</v>
       </c>
       <c r="E27" s="12">
-        <f t="shared" ref="E27:H27" si="14">D27</f>
+        <f t="shared" ref="E27:H27" si="13">D27</f>
         <v>2000</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2000</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2000</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="14">
-        <f t="shared" ref="B28" si="15">B14</f>
+        <f t="shared" ref="B28" si="14">B14</f>
         <v>0</v>
       </c>
       <c r="C28" s="14">
-        <f>C14</f>
+        <f t="shared" ref="C28:H28" si="15">C14</f>
         <v>-100</v>
       </c>
       <c r="D28" s="14">
-        <f>D14</f>
+        <f t="shared" si="15"/>
         <v>360</v>
       </c>
       <c r="E28" s="14">
-        <f>E14</f>
+        <f t="shared" si="15"/>
         <v>400</v>
       </c>
       <c r="F28" s="14">
-        <f>F14</f>
+        <f t="shared" si="15"/>
         <v>473.73333333333323</v>
       </c>
       <c r="G28" s="14">
-        <f>G14</f>
+        <f t="shared" si="15"/>
         <v>532.68266666666671</v>
       </c>
       <c r="H28" s="14">
-        <f>H14</f>
+        <f t="shared" si="15"/>
         <v>560</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>18</v>
       </c>
@@ -1490,7 +1516,7 @@
         <v>1666.4159999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16" thickBot="1">
+    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>14</v>
       </c>
@@ -1523,7 +1549,7 @@
         <v>3016.6666666666665</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>20</v>
       </c>
@@ -1549,7 +1575,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>21</v>
       </c>
@@ -1557,11 +1583,11 @@
         <v>0</v>
       </c>
       <c r="C32" s="14">
-        <f>B32-C39</f>
+        <f>B32-C45</f>
         <v>0</v>
       </c>
       <c r="D32" s="14">
-        <f t="shared" ref="D32:H32" si="18">C32-D39</f>
+        <f t="shared" ref="D32:H32" si="18">C32-D45</f>
         <v>0</v>
       </c>
       <c r="E32" s="14">
@@ -1581,272 +1607,297 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="23">
-        <f>C5/6</f>
+        <f t="shared" ref="C33:H33" si="19">C5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="D33" s="23">
-        <f>D5/6</f>
+        <f t="shared" si="19"/>
         <v>16.666666666666668</v>
       </c>
       <c r="E33" s="23">
-        <f>E5/6</f>
+        <f t="shared" si="19"/>
         <v>16.666666666666668</v>
       </c>
       <c r="F33" s="23">
-        <f>F5/6</f>
+        <f t="shared" si="19"/>
         <v>16.666666666666668</v>
       </c>
       <c r="G33" s="23">
-        <f>G5/6</f>
+        <f t="shared" si="19"/>
         <v>16.666666666666668</v>
       </c>
       <c r="H33" s="23">
-        <f>H5/6</f>
+        <f t="shared" si="19"/>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="16" thickBot="1">
+    <row r="34" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="10">
-        <f t="shared" ref="B34" si="19">B26+B30</f>
-        <v>0</v>
+        <f t="shared" ref="B34" si="20">B26+B30</f>
+        <v>2000</v>
       </c>
       <c r="C34" s="10">
-        <f t="shared" ref="C34:H34" si="20">C26+C30</f>
+        <f t="shared" ref="C34:H34" si="21">C26+C30</f>
         <v>10916.666666666666</v>
       </c>
       <c r="D34" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>10276.666666666668</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8833.3333333333358</v>
       </c>
       <c r="F34" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7833.3333333333339</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7683.0826666666662</v>
       </c>
       <c r="H34" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7243.0826666666653</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="16">
-        <f t="shared" ref="B35:H35" si="21">B25-B34</f>
+        <f t="shared" ref="B35:H35" si="22">B25-B34</f>
         <v>0</v>
       </c>
       <c r="C35" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="D35" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="E35" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F35" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G35" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H35" s="16">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="16">
-        <f>C19+C22+C23+B24-C26-C31-B32-C33</f>
-        <v>-916.66666666666663</v>
-      </c>
-      <c r="D38" s="16">
+      <c r="C44" s="16">
+        <f>C19+C22+C23-C26-C31-C33+B24-B32</f>
+        <v>1083.3333333333335</v>
+      </c>
+      <c r="D44" s="16">
         <f>D19+D22+D23+C24-D26-D31-C32-D33</f>
         <v>-26.666666666666668</v>
       </c>
-      <c r="E38" s="16">
-        <f t="shared" ref="E38:H38" si="22">E19+E22+E23+D24-E26-E31-D32-E33</f>
+      <c r="E44" s="16">
+        <f t="shared" ref="E44:H44" si="23">E19+E22+E23+D24-E26-E31-D32-E33</f>
         <v>1600.0000000000011</v>
       </c>
-      <c r="F38" s="16">
-        <f t="shared" si="22"/>
+      <c r="F44" s="16">
+        <f t="shared" si="23"/>
         <v>1526.2666666666657</v>
       </c>
-      <c r="G38" s="16">
-        <f t="shared" si="22"/>
+      <c r="G44" s="16">
+        <f t="shared" si="23"/>
         <v>-3532.6826666666666</v>
       </c>
-      <c r="H38" s="16">
-        <f t="shared" si="22"/>
+      <c r="H44" s="16">
+        <f t="shared" si="23"/>
         <v>-559.99999999999966</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="16">
-        <f>IF(C38&gt;=0,MIN(B32,-C38+MAX(C41,0)),MIN(B32,-C38))</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="16">
-        <f t="shared" ref="D39" si="23">IF(D38&gt;=0,MIN(C32,-D38+MAX(D41,0)),MIN(C32,-D38))</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="16">
-        <f t="shared" ref="E39" si="24">IF(E38&gt;=0,MIN(D32,-E38+MAX(E41,0)),MIN(D32,-E38))</f>
+      <c r="C45" s="16">
+        <f>IF(C44&gt;=0,MIN(B32,-C44+MAX(C46,0)),MIN(B32,-C44))</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="16">
+        <f>IF(D44&gt;=0,MIN(C32,-D44+MAX(D46,0)),MIN(C32,-D44))</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="16">
+        <f>IF(E44&gt;=0,MIN(D32,-E44+MAX(E46,0)),MIN(D32,-E44))</f>
         <v>-1156.6666666666679</v>
       </c>
-      <c r="F39" s="16">
-        <f t="shared" ref="F39:H39" si="25">IF(F38&gt;=0,MIN(E32,-F38+MAX(F41,0)),MIN(E32,-F38))</f>
+      <c r="F45" s="16">
+        <f>IF(F44&gt;=0,MIN(E32,-F44+MAX(F46,0)),MIN(E32,-F44))</f>
         <v>-1526.2666666666657</v>
       </c>
-      <c r="G39" s="16">
-        <f t="shared" si="25"/>
+      <c r="G45" s="16">
+        <f>IF(G44&gt;=0,MIN(F32,-G44+MAX(G46,0)),MIN(F32,-G44))</f>
         <v>2682.9333333333334</v>
       </c>
-      <c r="H39" s="16">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
+      <c r="H45" s="16">
+        <f>IF(H44&gt;=0,MIN(G32,-H44+MAX(H46,0)),MIN(G32,-H44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="16">
-        <f>IF(C38&gt;=0,MIN(C38,B24-$C$43),(C38+C39))</f>
-        <v>-916.66666666666663</v>
-      </c>
-      <c r="D41" s="16">
-        <f>IF(D38&gt;=0,MIN(D38,C24-$C$43),(D38+D39))</f>
+      <c r="C46" s="16">
+        <f>IF(C44&gt;=0,MIN(C44,B24-$C$47),(C44+C45))</f>
+        <v>1083.3333333333335</v>
+      </c>
+      <c r="D46" s="16">
+        <f>IF(D44&gt;=0,MIN(D44,C24-$C$47),(D44+D45))</f>
         <v>-26.666666666666668</v>
       </c>
-      <c r="E41" s="16">
-        <f>IF(E38&gt;=0,MIN(E38,D24-$C$43),(E38+E39))</f>
-        <v>443.33333333333326</v>
-      </c>
-      <c r="F41" s="16">
-        <f>IF(F38&gt;=0,MIN(F38,E24-$C$43),(F38+F39))</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="16">
-        <f>IF(G38&gt;=0,MIN(G38,F24-$C$43),(G38+G39))</f>
+      <c r="E46" s="16">
+        <f>IF(E44&gt;=0,MIN(E44,D24-$C$47),(E44+E45))</f>
+        <v>443.33333333333314</v>
+      </c>
+      <c r="F46" s="16">
+        <f>IF(F44&gt;=0,MIN(F44,E24-$C$47),(F44+F45))</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="16">
+        <f>IF(G44&gt;=0,MIN(G44,F24-$C$47),(G44+G45))</f>
         <v>-849.7493333333332</v>
       </c>
-      <c r="H41" s="16">
-        <f>IF(H38&gt;=0,MIN(H38,G24-$C$43),(H38+H39))</f>
+      <c r="H46" s="16">
+        <f>IF(H44&gt;=0,MIN(H44,G24-$C$47),(H44+H45))</f>
         <v>-559.99999999999966</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="24" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C47" s="24">
         <v>500</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16">
+      <c r="B50" s="16"/>
+      <c r="C50" s="16">
         <f>C14-(C20-B20)-(C22-B22)+(C33-B33)+C11-C24</f>
         <v>-11000</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D50" s="16">
         <f>D14-(D20-C20)-(D22-C22)+(D33-C33)+D11</f>
         <v>1476.6666666666667</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E50" s="16">
         <f>E14-(E20-D20)-(E22-D22)+(E33-D33)+E11</f>
         <v>1800</v>
       </c>
-      <c r="F46" s="16">
+      <c r="F50" s="16">
         <f>F14-(F20-E20)-(F22-E22)+(F33-E33)+F11</f>
         <v>1781.5666666666666</v>
       </c>
-      <c r="G46" s="16">
+      <c r="G50" s="16">
         <f>G14-(G20-F20)-(G22-F22)+(G33-F33)+G11</f>
         <v>1766.8293333333334</v>
       </c>
-      <c r="H46" s="16">
+      <c r="H50" s="16">
         <f>H14-(H20-G20)-(H22-G22)+(H33-G33)+H11</f>
         <v>1760</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16">
+      <c r="B51" s="16"/>
+      <c r="C51" s="16">
         <f>-(C27-B27)+C14+C9</f>
-        <v>-2100</v>
-      </c>
-      <c r="D47" s="16">
-        <f>-(D27-C27)-D41</f>
+        <v>-100</v>
+      </c>
+      <c r="D51" s="16">
+        <f>-(D27-C27)-D46</f>
         <v>26.666666666666668</v>
       </c>
-      <c r="E47" s="16">
-        <f t="shared" ref="E47:H47" si="26">-(E27-D27)-E41</f>
-        <v>-443.33333333333326</v>
-      </c>
-      <c r="F47" s="16">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="16">
-        <f t="shared" si="26"/>
+      <c r="E51" s="16">
+        <f>-(E27-D27)-E46</f>
+        <v>-443.33333333333314</v>
+      </c>
+      <c r="F51" s="16">
+        <f>-(F27-E27)-F46</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="16">
+        <f>-(G27-F27)-G46</f>
         <v>849.7493333333332</v>
       </c>
-      <c r="H47" s="16">
-        <f t="shared" si="26"/>
+      <c r="H51" s="16">
+        <f>-(H27-G27)-H46</f>
         <v>559.99999999999966</v>
       </c>
-      <c r="I47" s="16"/>
-    </row>
-    <row r="50" spans="5:5">
-      <c r="E50" s="16"/>
+      <c r="I51" s="16"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="16"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="26" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Revert previous excel model without my edits
</commit_message>
<xml_diff>
--- a/Specs/IS & BS.xlsx
+++ b/Specs/IS & BS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="15870" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140000" iterate="1" iterateCount="1000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>EBIT</t>
   </si>
@@ -133,21 +133,6 @@
   </si>
   <si>
     <t>day 1 of project start</t>
-  </si>
-  <si>
-    <t>fixed_assets+Operating Receivables + Short-Term Investments-  Equity - Lt_dept- St_dept_supl + PREVIOUS(Assets On Bank Accounts - ST_loans)</t>
-  </si>
-  <si>
-    <t>C14-(C20-B20)-(C22-B22)+(C33-B33)+C11-C24</t>
-  </si>
-  <si>
-    <t>Net earnings - CP_fixed_assets  - CP_Operating Receivables + CP_Short-Term Debt to Suppliers+C_Interests Paid-C_Assets On Bank Accounts</t>
-  </si>
-  <si>
-    <t>-(C27-B27)+C14+C9</t>
-  </si>
-  <si>
-    <t>- CP_Paid-In Capital+C_net_earn+C_Deprication</t>
   </si>
 </sst>
 </file>
@@ -200,15 +185,11 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -362,7 +343,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -430,36 +411,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -785,19 +758,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="40.875" customWidth="1"/>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -819,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -849,7 +822,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
@@ -871,7 +844,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
         <v>25</v>
       </c>
@@ -893,7 +866,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
@@ -923,7 +896,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -937,7 +910,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -959,7 +932,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -989,7 +962,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +984,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1014,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1044,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -1101,7 +1074,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -1131,7 +1104,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1161,16 +1134,16 @@
         <v>560</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
     </row>
-    <row r="18" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="37" thickBot="1">
       <c r="B18" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>8</v>
       </c>
@@ -1203,7 +1176,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="16" thickBot="1">
       <c r="A20" s="20" t="s">
         <v>30</v>
       </c>
@@ -1234,17 +1207,17 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="10">
         <f t="shared" ref="B21:H21" si="9">SUM(B22:B24)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C21" s="10">
         <f t="shared" si="9"/>
-        <v>916.66666666666652</v>
+        <v>916.66666666666663</v>
       </c>
       <c r="D21" s="10">
         <f t="shared" si="9"/>
@@ -1267,7 +1240,7 @@
         <v>2243.0826666666662</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="12" t="s">
         <v>10</v>
       </c>
@@ -1298,7 +1271,7 @@
         <v>333.33333333333331</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
         <v>11</v>
       </c>
@@ -1324,78 +1297,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="16" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="12">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C24" s="14">
-        <f>B24-C46</f>
-        <v>916.66666666666652</v>
+        <f>B24-C41</f>
+        <v>916.66666666666663</v>
       </c>
       <c r="D24" s="14">
-        <f>C24-D46</f>
-        <v>943.33333333333314</v>
+        <f t="shared" ref="D24:H24" si="10">C24-D41</f>
+        <v>943.33333333333326</v>
       </c>
       <c r="E24" s="14">
-        <f>D24-E46</f>
+        <f t="shared" si="10"/>
         <v>500</v>
       </c>
       <c r="F24" s="14">
-        <f>E24-F46</f>
+        <f t="shared" si="10"/>
         <v>500</v>
       </c>
       <c r="G24" s="14">
-        <f>F24-G46</f>
+        <f t="shared" si="10"/>
         <v>1349.7493333333332</v>
       </c>
       <c r="H24" s="14">
-        <f>G24-H46</f>
+        <f t="shared" si="10"/>
         <v>1909.7493333333327</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="16" thickBot="1">
       <c r="A25" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" ref="B25" si="10">B19+B21</f>
-        <v>2000</v>
+        <f t="shared" ref="B25" si="11">B19+B21</f>
+        <v>0</v>
       </c>
       <c r="C25" s="10">
-        <f t="shared" ref="C25:H25" si="11">C19+C21</f>
+        <f t="shared" ref="C25:H25" si="12">C19+C21</f>
         <v>10916.666666666666</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10276.666666666666</v>
       </c>
       <c r="E25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8833.3333333333339</v>
       </c>
       <c r="F25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7833.333333333333</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7683.0826666666662</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7243.0826666666662</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="16" thickBot="1">
       <c r="A26" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="10">
         <f>SUM(B27:B29)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C26" s="10">
         <f>SUM(C27:C29)</f>
@@ -1406,28 +1379,29 @@
         <v>2260</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" ref="E26:H26" si="12">SUM(E27:E29)</f>
+        <f t="shared" ref="E26:H26" si="13">SUM(E27:E29)</f>
         <v>2660</v>
       </c>
       <c r="F26" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3133.7333333333331</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3666.4159999999997</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4226.4159999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="12">
-        <v>2000</v>
+        <f>B24</f>
+        <v>0</v>
       </c>
       <c r="C27" s="12">
         <v>2000</v>
@@ -1437,56 +1411,56 @@
         <v>2000</v>
       </c>
       <c r="E27" s="12">
-        <f t="shared" ref="E27:H27" si="13">D27</f>
+        <f t="shared" ref="E27:H27" si="14">D27</f>
         <v>2000</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="14">
-        <f t="shared" ref="B28" si="14">B14</f>
+        <f t="shared" ref="B28" si="15">B14</f>
         <v>0</v>
       </c>
       <c r="C28" s="14">
-        <f t="shared" ref="C28:H28" si="15">C14</f>
+        <f>C14</f>
         <v>-100</v>
       </c>
       <c r="D28" s="14">
-        <f t="shared" si="15"/>
+        <f>D14</f>
         <v>360</v>
       </c>
       <c r="E28" s="14">
-        <f t="shared" si="15"/>
+        <f>E14</f>
         <v>400</v>
       </c>
       <c r="F28" s="14">
-        <f t="shared" si="15"/>
+        <f>F14</f>
         <v>473.73333333333323</v>
       </c>
       <c r="G28" s="14">
-        <f t="shared" si="15"/>
+        <f>G14</f>
         <v>532.68266666666671</v>
       </c>
       <c r="H28" s="14">
-        <f t="shared" si="15"/>
+        <f>H14</f>
         <v>560</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="12" t="s">
         <v>18</v>
       </c>
@@ -1516,7 +1490,7 @@
         <v>1666.4159999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="16" thickBot="1">
       <c r="A30" s="13" t="s">
         <v>14</v>
       </c>
@@ -1549,7 +1523,7 @@
         <v>3016.6666666666665</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="12" t="s">
         <v>20</v>
       </c>
@@ -1575,7 +1549,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="12" t="s">
         <v>21</v>
       </c>
@@ -1583,11 +1557,11 @@
         <v>0</v>
       </c>
       <c r="C32" s="14">
-        <f>B32-C45</f>
+        <f>B32-C39</f>
         <v>0</v>
       </c>
       <c r="D32" s="14">
-        <f t="shared" ref="D32:H32" si="18">C32-D45</f>
+        <f t="shared" ref="D32:H32" si="18">C32-D39</f>
         <v>0</v>
       </c>
       <c r="E32" s="14">
@@ -1607,297 +1581,272 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="23">
-        <f t="shared" ref="C33:H33" si="19">C5/6</f>
+        <f>C5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="D33" s="23">
-        <f t="shared" si="19"/>
+        <f>D5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="E33" s="23">
-        <f t="shared" si="19"/>
+        <f>E5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="F33" s="23">
-        <f t="shared" si="19"/>
+        <f>F5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="G33" s="23">
-        <f t="shared" si="19"/>
+        <f>G5/6</f>
         <v>16.666666666666668</v>
       </c>
       <c r="H33" s="23">
-        <f t="shared" si="19"/>
+        <f>H5/6</f>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="16" thickBot="1">
       <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="10">
-        <f t="shared" ref="B34" si="20">B26+B30</f>
-        <v>2000</v>
+        <f t="shared" ref="B34" si="19">B26+B30</f>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <f t="shared" ref="C34:H34" si="21">C26+C30</f>
+        <f t="shared" ref="C34:H34" si="20">C26+C30</f>
         <v>10916.666666666666</v>
       </c>
       <c r="D34" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>10276.666666666668</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8833.3333333333358</v>
       </c>
       <c r="F34" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>7833.3333333333339</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>7683.0826666666662</v>
       </c>
       <c r="H34" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>7243.0826666666653</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="16">
-        <f t="shared" ref="B35:H35" si="22">B25-B34</f>
+        <f t="shared" ref="B35:H35" si="21">B25-B34</f>
         <v>0</v>
       </c>
       <c r="C35" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="D35" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="E35" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F35" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G35" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H35" s="16">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="16">
-        <f>C19+C22+C23-C26-C31-C33+B24-B32</f>
-        <v>1083.3333333333335</v>
-      </c>
-      <c r="D44" s="16">
+      <c r="C38" s="16">
+        <f>C19+C22+C23+B24-C26-C31-B32-C33</f>
+        <v>-916.66666666666663</v>
+      </c>
+      <c r="D38" s="16">
         <f>D19+D22+D23+C24-D26-D31-C32-D33</f>
         <v>-26.666666666666668</v>
       </c>
-      <c r="E44" s="16">
-        <f t="shared" ref="E44:H44" si="23">E19+E22+E23+D24-E26-E31-D32-E33</f>
+      <c r="E38" s="16">
+        <f t="shared" ref="E38:H38" si="22">E19+E22+E23+D24-E26-E31-D32-E33</f>
         <v>1600.0000000000011</v>
       </c>
-      <c r="F44" s="16">
-        <f t="shared" si="23"/>
+      <c r="F38" s="16">
+        <f t="shared" si="22"/>
         <v>1526.2666666666657</v>
       </c>
-      <c r="G44" s="16">
-        <f t="shared" si="23"/>
+      <c r="G38" s="16">
+        <f t="shared" si="22"/>
         <v>-3532.6826666666666</v>
       </c>
-      <c r="H44" s="16">
-        <f t="shared" si="23"/>
+      <c r="H38" s="16">
+        <f t="shared" si="22"/>
         <v>-559.99999999999966</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="16">
-        <f>IF(C44&gt;=0,MIN(B32,-C44+MAX(C46,0)),MIN(B32,-C44))</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="16">
-        <f>IF(D44&gt;=0,MIN(C32,-D44+MAX(D46,0)),MIN(C32,-D44))</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="16">
-        <f>IF(E44&gt;=0,MIN(D32,-E44+MAX(E46,0)),MIN(D32,-E44))</f>
+      <c r="C39" s="16">
+        <f>IF(C38&gt;=0,MIN(B32,-C38+MAX(C41,0)),MIN(B32,-C38))</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" ref="D39" si="23">IF(D38&gt;=0,MIN(C32,-D38+MAX(D41,0)),MIN(C32,-D38))</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <f t="shared" ref="E39" si="24">IF(E38&gt;=0,MIN(D32,-E38+MAX(E41,0)),MIN(D32,-E38))</f>
         <v>-1156.6666666666679</v>
       </c>
-      <c r="F45" s="16">
-        <f>IF(F44&gt;=0,MIN(E32,-F44+MAX(F46,0)),MIN(E32,-F44))</f>
+      <c r="F39" s="16">
+        <f t="shared" ref="F39:H39" si="25">IF(F38&gt;=0,MIN(E32,-F38+MAX(F41,0)),MIN(E32,-F38))</f>
         <v>-1526.2666666666657</v>
       </c>
-      <c r="G45" s="16">
-        <f>IF(G44&gt;=0,MIN(F32,-G44+MAX(G46,0)),MIN(F32,-G44))</f>
+      <c r="G39" s="16">
+        <f t="shared" si="25"/>
         <v>2682.9333333333334</v>
       </c>
-      <c r="H45" s="16">
-        <f>IF(H44&gt;=0,MIN(G32,-H44+MAX(H46,0)),MIN(G32,-H44))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="16">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="16">
+        <f>IF(C38&gt;=0,MIN(C38,B24-$C$43),(C38+C39))</f>
+        <v>-916.66666666666663</v>
+      </c>
+      <c r="D41" s="16">
+        <f>IF(D38&gt;=0,MIN(D38,C24-$C$43),(D38+D39))</f>
+        <v>-26.666666666666668</v>
+      </c>
+      <c r="E41" s="16">
+        <f>IF(E38&gt;=0,MIN(E38,D24-$C$43),(E38+E39))</f>
+        <v>443.33333333333326</v>
+      </c>
+      <c r="F41" s="16">
+        <f>IF(F38&gt;=0,MIN(F38,E24-$C$43),(F38+F39))</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <f>IF(G38&gt;=0,MIN(G38,F24-$C$43),(G38+G39))</f>
+        <v>-849.7493333333332</v>
+      </c>
+      <c r="H41" s="16">
+        <f>IF(H38&gt;=0,MIN(H38,G24-$C$43),(H38+H39))</f>
+        <v>-559.99999999999966</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>33</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B46" s="16"/>
       <c r="C46" s="16">
-        <f>IF(C44&gt;=0,MIN(C44,B24-$C$47),(C44+C45))</f>
-        <v>1083.3333333333335</v>
-      </c>
-      <c r="D46" s="16">
-        <f>IF(D44&gt;=0,MIN(D44,C24-$C$47),(D44+D45))</f>
-        <v>-26.666666666666668</v>
-      </c>
-      <c r="E46" s="16">
-        <f>IF(E44&gt;=0,MIN(E44,D24-$C$47),(E44+E45))</f>
-        <v>443.33333333333314</v>
-      </c>
-      <c r="F46" s="16">
-        <f>IF(F44&gt;=0,MIN(F44,E24-$C$47),(F44+F45))</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="16">
-        <f>IF(G44&gt;=0,MIN(G44,F24-$C$47),(G44+G45))</f>
-        <v>-849.7493333333332</v>
-      </c>
-      <c r="H46" s="16">
-        <f>IF(H44&gt;=0,MIN(H44,G24-$C$47),(H44+H45))</f>
-        <v>-559.99999999999966</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="24">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16">
         <f>C14-(C20-B20)-(C22-B22)+(C33-B33)+C11-C24</f>
         <v>-11000</v>
       </c>
-      <c r="D50" s="16">
+      <c r="D46" s="16">
         <f>D14-(D20-C20)-(D22-C22)+(D33-C33)+D11</f>
         <v>1476.6666666666667</v>
       </c>
-      <c r="E50" s="16">
+      <c r="E46" s="16">
         <f>E14-(E20-D20)-(E22-D22)+(E33-D33)+E11</f>
         <v>1800</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F46" s="16">
         <f>F14-(F20-E20)-(F22-E22)+(F33-E33)+F11</f>
         <v>1781.5666666666666</v>
       </c>
-      <c r="G50" s="16">
+      <c r="G46" s="16">
         <f>G14-(G20-F20)-(G22-F22)+(G33-F33)+G11</f>
         <v>1766.8293333333334</v>
       </c>
-      <c r="H50" s="16">
+      <c r="H46" s="16">
         <f>H14-(H20-G20)-(H22-G22)+(H33-G33)+H11</f>
         <v>1760</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16">
+      <c r="B47" s="16"/>
+      <c r="C47" s="16">
         <f>-(C27-B27)+C14+C9</f>
-        <v>-100</v>
-      </c>
-      <c r="D51" s="16">
-        <f>-(D27-C27)-D46</f>
+        <v>-2100</v>
+      </c>
+      <c r="D47" s="16">
+        <f>-(D27-C27)-D41</f>
         <v>26.666666666666668</v>
       </c>
-      <c r="E51" s="16">
-        <f>-(E27-D27)-E46</f>
-        <v>-443.33333333333314</v>
-      </c>
-      <c r="F51" s="16">
-        <f>-(F27-E27)-F46</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="16">
-        <f>-(G27-F27)-G46</f>
+      <c r="E47" s="16">
+        <f t="shared" ref="E47:H47" si="26">-(E27-D27)-E41</f>
+        <v>-443.33333333333326</v>
+      </c>
+      <c r="F47" s="16">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <f t="shared" si="26"/>
         <v>849.7493333333332</v>
       </c>
-      <c r="H51" s="16">
-        <f>-(H27-G27)-H46</f>
+      <c r="H47" s="16">
+        <f t="shared" si="26"/>
         <v>559.99999999999966</v>
       </c>
-      <c r="I51" s="16"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E54" s="16"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="26" t="s">
-        <v>42</v>
-      </c>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>